<commit_message>
EFQ with average instead of sum for subscales
</commit_message>
<xml_diff>
--- a/scoresheets_tocheck/EFQ_Scoresheet.xlsx
+++ b/scoresheets_tocheck/EFQ_Scoresheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenpictor/Desktop/BAM-data-cleaning/scoresheets_tocheck/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE44853F-D338-3349-B019-2815B616063E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C859CF3-7CB2-AE48-BAD6-489EC845E9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15740" xr2:uid="{997E3381-58D2-8F42-82F4-13846D810F39}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="109">
   <si>
     <t>raw_vars</t>
   </si>
@@ -320,106 +320,49 @@
     <t>efq_1_wt_gain, efq_2_gain_afraid</t>
   </si>
   <si>
-    <t>sum of EFQ Fear of Weight Gain questions</t>
-  </si>
-  <si>
     <t>efq_3_rejected, efq_4_disappoint, efq_5_judged, efq_6_look_funny, efq_7_criticize, efq_8_judged_eat, efq_9_abandon, efq_10_perfect</t>
   </si>
   <si>
     <t>efq_fosc</t>
   </si>
   <si>
-    <t>sum of EFQ Fear of Social Consequences questions</t>
-  </si>
-  <si>
     <t>efq_11_overeat_lazy, efq_14_lose_calorie, efq_15_afraid_full, efq_16_life_weight, efq_17_cant_control</t>
   </si>
   <si>
     <t>efq_fopc</t>
   </si>
   <si>
-    <t>sum of EFQ Fear of Personal Consequences questions</t>
-  </si>
-  <si>
     <t>efq_13_emotion_weight, efq_18_uncomfortable, efq_19_not_like</t>
   </si>
   <si>
     <t>efq_fops</t>
   </si>
   <si>
-    <t>sum of EFQ Fear of Physical Sensations questions</t>
-  </si>
-  <si>
     <t>efq_12_public, efq_20_eating_front</t>
   </si>
   <si>
     <t>efq_fose</t>
   </si>
   <si>
-    <t>sum of EFQ Fear of Social Eating questions</t>
-  </si>
-  <si>
     <t>efq_fowg</t>
   </si>
   <si>
-    <t>efq_fowg_weighted_sum</t>
-  </si>
-  <si>
-    <t>efq_fowg_sum_25</t>
-  </si>
-  <si>
-    <t>weighted sum of EFQ FOWG with 25% or less missing</t>
-  </si>
-  <si>
-    <t>efq_fowg_NA_percent &gt; 25</t>
-  </si>
-  <si>
-    <t>efq_fosc_weighted_sum</t>
-  </si>
-  <si>
-    <t>efq_fosc_sum_25</t>
-  </si>
-  <si>
-    <t>weighted sum of EFQ FOSC with 25% or less missing</t>
-  </si>
-  <si>
-    <t>efq_fosc_NA_percent &gt; 25</t>
-  </si>
-  <si>
-    <t>efq_fopc_weighted_sum</t>
-  </si>
-  <si>
-    <t>weighted sum of EFQ FOPC with 25% or less missing</t>
-  </si>
-  <si>
-    <t>efq_fopc_NA_percent &gt; 25</t>
-  </si>
-  <si>
-    <t>efq_fops_weighted_sum</t>
-  </si>
-  <si>
-    <t>efq_fopc_sum_25</t>
-  </si>
-  <si>
-    <t>efq_fops_sum_25</t>
-  </si>
-  <si>
-    <t>weighted sum of EFQ FOPS with 25% or less missing</t>
-  </si>
-  <si>
-    <t>efq_fops_NA_percent &gt; 25</t>
-  </si>
-  <si>
-    <t>efq_fose_weighted_sum</t>
-  </si>
-  <si>
-    <t>efq_fose_sum_25</t>
-  </si>
-  <si>
-    <t>weighted sum of EFQ FOSE with 25% or less missing</t>
-  </si>
-  <si>
-    <t>efq_fose_NA_percent &gt; 25</t>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>average of EFQ Fear of Weight Gain questions</t>
+  </si>
+  <si>
+    <t>average of EFQ Fear of Social Consequences questions</t>
+  </si>
+  <si>
+    <t>average of EFQ Fear of Personal Consequences questions</t>
+  </si>
+  <si>
+    <t>average of EFQ Fear of Physical Sensations questions</t>
+  </si>
+  <si>
+    <t>average of EFQ Fear of Social Eating questions</t>
   </si>
 </sst>
 </file>
@@ -784,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7308F9-F148-F248-A8CF-73AEFF3C6044}">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2485,13 +2428,13 @@
         <v>93</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="E49" s="1">
         <v>4</v>
@@ -2517,16 +2460,16 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="C50" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="E50" s="1">
         <v>4</v>
@@ -2556,16 +2499,16 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="E51" s="1">
         <v>4</v>
@@ -2591,16 +2534,16 @@
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="E52" s="1">
         <v>4</v>
@@ -2626,16 +2569,16 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="E53" s="1">
         <v>4</v>
@@ -2691,181 +2634,6 @@
         <v>91</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A55" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E55" s="1">
-        <v>5</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J55" t="s">
-        <v>91</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E56" s="1">
-        <v>5</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J56" t="s">
-        <v>91</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E57" s="1">
-        <v>5</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J57" t="s">
-        <v>91</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E58" s="1">
-        <v>5</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J58" t="s">
-        <v>91</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E59" s="1">
-        <v>5</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J59" t="s">
-        <v>91</v>
-      </c>
-      <c r="K59" s="1" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>